<commit_message>
Updating the Final Code
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github_Code\webShopDemo\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD8F3595-3313-461E-9A2A-149EEF26E600}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1F1FF1-CFFC-48C3-A37B-526810D15221}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="2840" windowWidth="14400" windowHeight="7360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -208,13 +208,7 @@
   </si>
   <si>
     <t>Welcome, Please Sign In! is verified successfully._x000D_
-atest@gmail.com is verified successfully._x000D_
-Message displayed Your Shopping Cart is empty! _x000D_
-Item Price: '51.00 ' retrieved from the itemCart_x000D_
-subTotal: 510.00 and ItemTotal:510 are matched._x000D_
-Paymentinformation verification is success. Payment info message is You will pay by COD_x000D_
-Order status verification is success. Order status message is Your order has been successfully processed!_x000D_
-Order Number generated. Order Number is 790322</t>
+atest@gmail.com is verified successfully.</t>
   </si>
 </sst>
 </file>
@@ -660,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A31373E-4625-4B95-8FE7-62CBCF15DF6D}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -697,7 +691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -708,12 +702,17 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -731,7 +730,6 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -749,7 +747,6 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -767,7 +764,6 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -785,9 +781,8 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="261" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -798,16 +793,10 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -885,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55844BD-BB9C-4B5B-8F46-E3B81B5A3FEC}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>